<commit_message>
Use Apache POI instead of SX.jar
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingxiao\Documents\GitHub\PageRank\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="5520" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="5520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,74 +19,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>http://evget.com</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
   <si>
     <t>http://pda.memori.ru</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>http://socialbookmarkssite.com</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>http://www.codepool.biz</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="9" formatCode="0%"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="64"/>
       <name val="宋体"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="64"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color indexed="64"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <color indexed="64"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="64"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11"/>
@@ -90,8 +51,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,92 +78,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="bottom" horizontal="general"/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -205,10 +104,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -243,7 +142,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -278,7 +177,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -366,7 +265,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -375,13 +274,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -391,7 +290,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -400,7 +299,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -409,7 +308,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -419,12 +318,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -455,7 +354,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -474,7 +373,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -486,48 +385,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="n">
+        <v>4.0</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="21" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B3" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>7</v>
+      <c r="B4" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>